<commit_message>
changed calculation for infiltration
</commit_message>
<xml_diff>
--- a/raw_inputs/vent.xlsx
+++ b/raw_inputs/vent.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tec_params" sheetId="1" r:id="rId1"/>
     <sheet name="sci_params" sheetId="3" r:id="rId2"/>
     <sheet name="eco_params" sheetId="2" r:id="rId3"/>
+    <sheet name="n_50_table" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>m³/kg</t>
   </si>
@@ -120,12 +121,42 @@
   </si>
   <si>
     <t>heat capacity air</t>
+  </si>
+  <si>
+    <t>n_50</t>
+  </si>
+  <si>
+    <t>x_vent</t>
+  </si>
+  <si>
+    <t>SFH</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>retrofit</t>
+  </si>
+  <si>
+    <t>MFH</t>
+  </si>
+  <si>
+    <t>Rooftop</t>
+  </si>
+  <si>
+    <t>adv_retr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,15 +166,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -151,12 +194,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -439,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -492,7 +603,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -593,7 +704,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,4 +772,1834 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0</v>
+      </c>
+      <c r="O10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11">
+        <v>2</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>0</v>
+      </c>
+      <c r="O13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
+      <c r="N14" s="12">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0</v>
+      </c>
+      <c r="L15" s="9">
+        <v>0</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0</v>
+      </c>
+      <c r="O15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
+        <v>0</v>
+      </c>
+      <c r="N16" s="12">
+        <v>0</v>
+      </c>
+      <c r="O16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>14</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>15</v>
+      </c>
+      <c r="B18" s="11">
+        <v>2</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
+        <v>0</v>
+      </c>
+      <c r="N18" s="12">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+      <c r="N19" s="9">
+        <v>0</v>
+      </c>
+      <c r="O19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11">
+        <v>2</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20" s="12">
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0</v>
+      </c>
+      <c r="O21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>19</v>
+      </c>
+      <c r="B22" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>1</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <v>1</v>
+      </c>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22" s="12">
+        <v>0</v>
+      </c>
+      <c r="O22" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>20</v>
+      </c>
+      <c r="B23" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="9">
+        <v>1</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0</v>
+      </c>
+      <c r="O23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>21</v>
+      </c>
+      <c r="B24" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <v>1</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12">
+        <v>1</v>
+      </c>
+      <c r="N24" s="12">
+        <v>0</v>
+      </c>
+      <c r="O24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>22</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>1</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
+      <c r="N25" s="9">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>23</v>
+      </c>
+      <c r="B26" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <v>1</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12">
+        <v>1</v>
+      </c>
+      <c r="N26" s="12">
+        <v>0</v>
+      </c>
+      <c r="O26" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>24</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>25</v>
+      </c>
+      <c r="B28" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0</v>
+      </c>
+      <c r="D28" s="12">
+        <v>0</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0</v>
+      </c>
+      <c r="J28" s="12">
+        <v>1</v>
+      </c>
+      <c r="K28" s="12">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1</v>
+      </c>
+      <c r="M28" s="12">
+        <v>0</v>
+      </c>
+      <c r="N28" s="12">
+        <v>0</v>
+      </c>
+      <c r="O28" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>26</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>1</v>
+      </c>
+      <c r="L29" s="9">
+        <v>1</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>27</v>
+      </c>
+      <c r="B30" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0</v>
+      </c>
+      <c r="I30" s="12">
+        <v>0</v>
+      </c>
+      <c r="J30" s="12">
+        <v>1</v>
+      </c>
+      <c r="K30" s="12">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <v>1</v>
+      </c>
+      <c r="M30" s="12">
+        <v>0</v>
+      </c>
+      <c r="N30" s="12">
+        <v>0</v>
+      </c>
+      <c r="O30" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>28</v>
+      </c>
+      <c r="B31" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0</v>
+      </c>
+      <c r="I31" s="9">
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+      <c r="K31" s="9">
+        <v>1</v>
+      </c>
+      <c r="L31" s="9">
+        <v>1</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0</v>
+      </c>
+      <c r="O31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>29</v>
+      </c>
+      <c r="B32" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0</v>
+      </c>
+      <c r="G32" s="12">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <v>0</v>
+      </c>
+      <c r="J32" s="12">
+        <v>1</v>
+      </c>
+      <c r="K32" s="12">
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
+        <v>0</v>
+      </c>
+      <c r="M32" s="12">
+        <v>1</v>
+      </c>
+      <c r="N32" s="12">
+        <v>0</v>
+      </c>
+      <c r="O32" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>30</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
+        <v>1</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
+      <c r="N33" s="9">
+        <v>1</v>
+      </c>
+      <c r="O33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>31</v>
+      </c>
+      <c r="B34" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12">
+        <v>0</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
+        <v>1</v>
+      </c>
+      <c r="L34" s="12">
+        <v>0</v>
+      </c>
+      <c r="M34" s="12">
+        <v>1</v>
+      </c>
+      <c r="N34" s="12">
+        <v>0</v>
+      </c>
+      <c r="O34" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>32</v>
+      </c>
+      <c r="B35" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="9">
+        <v>0</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0</v>
+      </c>
+      <c r="K35" s="9">
+        <v>1</v>
+      </c>
+      <c r="L35" s="9">
+        <v>0</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>1</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>33</v>
+      </c>
+      <c r="B36" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0</v>
+      </c>
+      <c r="I36" s="12">
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <v>1</v>
+      </c>
+      <c r="K36" s="12">
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
+        <v>0</v>
+      </c>
+      <c r="M36" s="12">
+        <v>1</v>
+      </c>
+      <c r="N36" s="12">
+        <v>0</v>
+      </c>
+      <c r="O36" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>34</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0</v>
+      </c>
+      <c r="I37" s="9">
+        <v>0</v>
+      </c>
+      <c r="J37" s="9">
+        <v>1</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
+      </c>
+      <c r="N37" s="9">
+        <v>1</v>
+      </c>
+      <c r="O37" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>35</v>
+      </c>
+      <c r="B38" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
+        <v>0</v>
+      </c>
+      <c r="J38" s="12">
+        <v>0</v>
+      </c>
+      <c r="K38" s="12">
+        <v>1</v>
+      </c>
+      <c r="L38" s="12">
+        <v>0</v>
+      </c>
+      <c r="M38" s="12">
+        <v>1</v>
+      </c>
+      <c r="N38" s="12">
+        <v>0</v>
+      </c>
+      <c r="O38" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>36</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="9">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <v>0</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0</v>
+      </c>
+      <c r="I39" s="9">
+        <v>0</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0</v>
+      </c>
+      <c r="K39" s="9">
+        <v>1</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>1</v>
+      </c>
+      <c r="O39" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
latest version with problem of wrong unit (kWh instead of Wh)
</commit_message>
<xml_diff>
--- a/raw_inputs/vent.xlsx
+++ b/raw_inputs/vent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tec_params" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="eco_params" sheetId="2" r:id="rId3"/>
     <sheet name="n_50_table" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
-    <t>m³/kg</t>
-  </si>
-  <si>
     <t>cp_air</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>adv_retr</t>
+  </si>
+  <si>
+    <t>kg/m³</t>
   </si>
 </sst>
 </file>
@@ -551,62 +551,62 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>0.15</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0.05</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -618,80 +618,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1.204</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>1.0049999999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
       </c>
       <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -715,58 +715,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>79.13</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>-0.35</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -778,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
@@ -803,7 +803,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
@@ -811,7 +811,7 @@
       <c r="G1" s="14"/>
       <c r="H1" s="6"/>
       <c r="I1" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
@@ -821,85 +821,85 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added multiple run to get vent data + u-values successfully changed vent modelation in building_optimization maybe ajustment in u-values necessary
</commit_message>
<xml_diff>
--- a/raw_inputs/vent.xlsx
+++ b/raw_inputs/vent.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_CBB0F254D61FAC46654419B56F41A41CBA152627" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BEA42060-53FC-4F57-8FCE-6C85DB1C084C}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tec_params" sheetId="1" r:id="rId1"/>
     <sheet name="sci_params" sheetId="3" r:id="rId2"/>
     <sheet name="eco_params" sheetId="2" r:id="rId3"/>
-    <sheet name="n_50_table" sheetId="4" r:id="rId4"/>
+    <sheet name="n_50_table_1957" sheetId="4" r:id="rId4"/>
+    <sheet name="n_50_table_1978" sheetId="5" r:id="rId5"/>
+    <sheet name="n_50_table_1994" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
   <si>
     <t>cp_air</t>
   </si>
@@ -195,7 +196,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -284,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -307,6 +308,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -589,16 +593,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -612,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -626,12 +630,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -640,7 +644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -657,16 +661,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" activeCellId="1" sqref="H22 D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -680,7 +684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -694,7 +698,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -708,7 +712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -722,7 +726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -736,7 +740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -750,7 +754,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -764,12 +768,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8">
-        <v>2.5</v>
+        <v>1.3</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
@@ -778,12 +782,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
       <c r="B9">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -792,13 +796,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
       <c r="B10">
         <f>LN(B8/B9)/LN(80/B9)</f>
-        <v>0.34587989676093622</v>
+        <v>0.26250218690605115</v>
       </c>
     </row>
   </sheetData>
@@ -807,20 +811,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -834,7 +838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -848,7 +852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -862,7 +866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -882,51 +886,3711 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0</v>
+      </c>
+      <c r="O10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>0</v>
+      </c>
+      <c r="O13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
+      <c r="N14" s="12">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0</v>
+      </c>
+      <c r="L15" s="9">
+        <v>0</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0</v>
+      </c>
+      <c r="O15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
+        <v>0</v>
+      </c>
+      <c r="N16" s="12">
+        <v>0</v>
+      </c>
+      <c r="O16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>14</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>15</v>
+      </c>
+      <c r="B18" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
+        <v>0</v>
+      </c>
+      <c r="N18" s="12">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+      <c r="N19" s="9">
+        <v>0</v>
+      </c>
+      <c r="O19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20" s="12">
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0</v>
+      </c>
+      <c r="O21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>19</v>
+      </c>
+      <c r="B22" s="11">
+        <v>10</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>1</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <v>1</v>
+      </c>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22" s="12">
+        <v>0</v>
+      </c>
+      <c r="O22" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>20</v>
+      </c>
+      <c r="B23" s="8">
+        <v>10</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="9">
+        <v>1</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0</v>
+      </c>
+      <c r="O23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>21</v>
+      </c>
+      <c r="B24" s="11">
+        <v>4</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <v>1</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12">
+        <v>1</v>
+      </c>
+      <c r="N24" s="12">
+        <v>0</v>
+      </c>
+      <c r="O24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>22</v>
+      </c>
+      <c r="B25" s="8">
+        <v>4</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>1</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
+      <c r="N25" s="9">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>23</v>
+      </c>
+      <c r="B26" s="11">
+        <v>4</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <v>1</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12">
+        <v>1</v>
+      </c>
+      <c r="N26" s="12">
+        <v>0</v>
+      </c>
+      <c r="O26" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>24</v>
+      </c>
+      <c r="B27" s="8">
+        <v>4</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>25</v>
+      </c>
+      <c r="B28" s="11">
+        <v>4</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0</v>
+      </c>
+      <c r="D28" s="12">
+        <v>0</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0</v>
+      </c>
+      <c r="J28" s="12">
+        <v>1</v>
+      </c>
+      <c r="K28" s="12">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1</v>
+      </c>
+      <c r="M28" s="12">
+        <v>0</v>
+      </c>
+      <c r="N28" s="12">
+        <v>0</v>
+      </c>
+      <c r="O28" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>26</v>
+      </c>
+      <c r="B29" s="8">
+        <v>4</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>1</v>
+      </c>
+      <c r="L29" s="9">
+        <v>1</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>27</v>
+      </c>
+      <c r="B30" s="11">
+        <v>4</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0</v>
+      </c>
+      <c r="I30" s="12">
+        <v>0</v>
+      </c>
+      <c r="J30" s="12">
+        <v>1</v>
+      </c>
+      <c r="K30" s="12">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <v>1</v>
+      </c>
+      <c r="M30" s="12">
+        <v>0</v>
+      </c>
+      <c r="N30" s="12">
+        <v>0</v>
+      </c>
+      <c r="O30" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>28</v>
+      </c>
+      <c r="B31" s="8">
+        <v>4</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0</v>
+      </c>
+      <c r="I31" s="9">
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+      <c r="K31" s="9">
+        <v>1</v>
+      </c>
+      <c r="L31" s="9">
+        <v>1</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0</v>
+      </c>
+      <c r="O31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>29</v>
+      </c>
+      <c r="B32" s="11">
+        <v>4</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0</v>
+      </c>
+      <c r="G32" s="12">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <v>0</v>
+      </c>
+      <c r="J32" s="12">
+        <v>1</v>
+      </c>
+      <c r="K32" s="12">
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
+        <v>0</v>
+      </c>
+      <c r="M32" s="12">
+        <v>1</v>
+      </c>
+      <c r="N32" s="12">
+        <v>0</v>
+      </c>
+      <c r="O32" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>30</v>
+      </c>
+      <c r="B33" s="8">
+        <v>2</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
+        <v>1</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
+      <c r="N33" s="9">
+        <v>1</v>
+      </c>
+      <c r="O33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>31</v>
+      </c>
+      <c r="B34" s="11">
+        <v>2</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12">
+        <v>0</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
+        <v>1</v>
+      </c>
+      <c r="L34" s="12">
+        <v>0</v>
+      </c>
+      <c r="M34" s="12">
+        <v>1</v>
+      </c>
+      <c r="N34" s="12">
+        <v>0</v>
+      </c>
+      <c r="O34" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>32</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="9">
+        <v>0</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0</v>
+      </c>
+      <c r="K35" s="9">
+        <v>1</v>
+      </c>
+      <c r="L35" s="9">
+        <v>0</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>1</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>33</v>
+      </c>
+      <c r="B36" s="11">
+        <v>4</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0</v>
+      </c>
+      <c r="I36" s="12">
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <v>1</v>
+      </c>
+      <c r="K36" s="12">
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
+        <v>0</v>
+      </c>
+      <c r="M36" s="12">
+        <v>1</v>
+      </c>
+      <c r="N36" s="12">
+        <v>0</v>
+      </c>
+      <c r="O36" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>34</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0</v>
+      </c>
+      <c r="I37" s="9">
+        <v>0</v>
+      </c>
+      <c r="J37" s="9">
+        <v>1</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
+      </c>
+      <c r="N37" s="9">
+        <v>1</v>
+      </c>
+      <c r="O37" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>35</v>
+      </c>
+      <c r="B38" s="11">
+        <v>1</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
+        <v>0</v>
+      </c>
+      <c r="J38" s="12">
+        <v>0</v>
+      </c>
+      <c r="K38" s="12">
+        <v>1</v>
+      </c>
+      <c r="L38" s="12">
+        <v>0</v>
+      </c>
+      <c r="M38" s="12">
+        <v>1</v>
+      </c>
+      <c r="N38" s="12">
+        <v>0</v>
+      </c>
+      <c r="O38" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>36</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="9">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <v>0</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0</v>
+      </c>
+      <c r="I39" s="9">
+        <v>0</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0</v>
+      </c>
+      <c r="K39" s="9">
+        <v>1</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>1</v>
+      </c>
+      <c r="O39" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>11.41</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>11.41</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0</v>
+      </c>
+      <c r="O10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>0</v>
+      </c>
+      <c r="O13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
+      <c r="N14" s="12">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0</v>
+      </c>
+      <c r="L15" s="9">
+        <v>0</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0</v>
+      </c>
+      <c r="O15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
+        <v>0</v>
+      </c>
+      <c r="N16" s="12">
+        <v>0</v>
+      </c>
+      <c r="O16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>14</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0</v>
+      </c>
+      <c r="O17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>15</v>
+      </c>
+      <c r="B18" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
+        <v>0</v>
+      </c>
+      <c r="N18" s="12">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+      <c r="N19" s="9">
+        <v>0</v>
+      </c>
+      <c r="O19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20" s="12">
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0</v>
+      </c>
+      <c r="O21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>19</v>
+      </c>
+      <c r="B22" s="11">
+        <v>5.41</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>1</v>
+      </c>
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <v>1</v>
+      </c>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22" s="12">
+        <v>0</v>
+      </c>
+      <c r="O22" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>20</v>
+      </c>
+      <c r="B23" s="8">
+        <v>5.41</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="9">
+        <v>1</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0</v>
+      </c>
+      <c r="O23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>21</v>
+      </c>
+      <c r="B24" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <v>1</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12">
+        <v>1</v>
+      </c>
+      <c r="N24" s="12">
+        <v>0</v>
+      </c>
+      <c r="O24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>22</v>
+      </c>
+      <c r="B25" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>1</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0</v>
+      </c>
+      <c r="N25" s="9">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>23</v>
+      </c>
+      <c r="B26" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <v>1</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12">
+        <v>1</v>
+      </c>
+      <c r="N26" s="12">
+        <v>0</v>
+      </c>
+      <c r="O26" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>24</v>
+      </c>
+      <c r="B27" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>25</v>
+      </c>
+      <c r="B28" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0</v>
+      </c>
+      <c r="D28" s="12">
+        <v>0</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0</v>
+      </c>
+      <c r="J28" s="12">
+        <v>1</v>
+      </c>
+      <c r="K28" s="12">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1</v>
+      </c>
+      <c r="M28" s="12">
+        <v>0</v>
+      </c>
+      <c r="N28" s="12">
+        <v>0</v>
+      </c>
+      <c r="O28" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>26</v>
+      </c>
+      <c r="B29" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>1</v>
+      </c>
+      <c r="L29" s="9">
+        <v>1</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>27</v>
+      </c>
+      <c r="B30" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0</v>
+      </c>
+      <c r="I30" s="12">
+        <v>0</v>
+      </c>
+      <c r="J30" s="12">
+        <v>1</v>
+      </c>
+      <c r="K30" s="12">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <v>1</v>
+      </c>
+      <c r="M30" s="12">
+        <v>0</v>
+      </c>
+      <c r="N30" s="12">
+        <v>0</v>
+      </c>
+      <c r="O30" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>28</v>
+      </c>
+      <c r="B31" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
+        <v>0</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0</v>
+      </c>
+      <c r="I31" s="9">
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
+      <c r="K31" s="9">
+        <v>1</v>
+      </c>
+      <c r="L31" s="9">
+        <v>1</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0</v>
+      </c>
+      <c r="O31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>29</v>
+      </c>
+      <c r="B32" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0</v>
+      </c>
+      <c r="G32" s="12">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <v>0</v>
+      </c>
+      <c r="J32" s="12">
+        <v>1</v>
+      </c>
+      <c r="K32" s="12">
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
+        <v>0</v>
+      </c>
+      <c r="M32" s="12">
+        <v>1</v>
+      </c>
+      <c r="N32" s="12">
+        <v>0</v>
+      </c>
+      <c r="O32" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>30</v>
+      </c>
+      <c r="B33" s="8">
+        <v>2</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
+        <v>1</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0</v>
+      </c>
+      <c r="N33" s="9">
+        <v>1</v>
+      </c>
+      <c r="O33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>31</v>
+      </c>
+      <c r="B34" s="11">
+        <v>2</v>
+      </c>
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12">
+        <v>0</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
+        <v>1</v>
+      </c>
+      <c r="L34" s="12">
+        <v>0</v>
+      </c>
+      <c r="M34" s="12">
+        <v>1</v>
+      </c>
+      <c r="N34" s="12">
+        <v>0</v>
+      </c>
+      <c r="O34" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>32</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="9">
+        <v>0</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0</v>
+      </c>
+      <c r="K35" s="9">
+        <v>1</v>
+      </c>
+      <c r="L35" s="9">
+        <v>0</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>1</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>33</v>
+      </c>
+      <c r="B36" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0</v>
+      </c>
+      <c r="I36" s="12">
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <v>1</v>
+      </c>
+      <c r="K36" s="12">
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
+        <v>0</v>
+      </c>
+      <c r="M36" s="12">
+        <v>1</v>
+      </c>
+      <c r="N36" s="12">
+        <v>0</v>
+      </c>
+      <c r="O36" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>34</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0</v>
+      </c>
+      <c r="I37" s="9">
+        <v>0</v>
+      </c>
+      <c r="J37" s="9">
+        <v>1</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
+      </c>
+      <c r="N37" s="9">
+        <v>1</v>
+      </c>
+      <c r="O37" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>35</v>
+      </c>
+      <c r="B38" s="11">
+        <v>1</v>
+      </c>
+      <c r="C38" s="12">
+        <v>0</v>
+      </c>
+      <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
+        <v>0</v>
+      </c>
+      <c r="J38" s="12">
+        <v>0</v>
+      </c>
+      <c r="K38" s="12">
+        <v>1</v>
+      </c>
+      <c r="L38" s="12">
+        <v>0</v>
+      </c>
+      <c r="M38" s="12">
+        <v>1</v>
+      </c>
+      <c r="N38" s="12">
+        <v>0</v>
+      </c>
+      <c r="O38" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>36</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="9">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <v>0</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0</v>
+      </c>
+      <c r="I39" s="9">
+        <v>0</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0</v>
+      </c>
+      <c r="K39" s="9">
+        <v>1</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>1</v>
+      </c>
+      <c r="O39" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.265625" customWidth="1"/>
-    <col min="6" max="6" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.265625" customWidth="1"/>
-    <col min="12" max="12" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.265625" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -964,7 +4628,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>32</v>
@@ -1009,59 +4673,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="5">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -1103,12 +4767,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>3</v>
       </c>
       <c r="B6" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -1150,12 +4814,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="8">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -1197,12 +4861,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>5</v>
       </c>
       <c r="B8" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
@@ -1244,12 +4908,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="8">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -1291,12 +4955,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>7</v>
       </c>
       <c r="B10" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C10" s="12">
         <v>0</v>
@@ -1338,12 +5002,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
       <c r="B11" s="8">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
@@ -1385,12 +5049,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>9</v>
       </c>
       <c r="B12" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C12" s="12">
         <v>0</v>
@@ -1432,12 +5096,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
       <c r="B13" s="8">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
@@ -1479,12 +5143,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>11</v>
       </c>
       <c r="B14" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C14" s="12">
         <v>0</v>
@@ -1526,12 +5190,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>12</v>
       </c>
       <c r="B15" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1573,12 +5237,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>13</v>
       </c>
       <c r="B16" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="12">
         <v>0</v>
@@ -1620,12 +5284,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>14</v>
       </c>
       <c r="B17" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
@@ -1667,12 +5331,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>15</v>
       </c>
       <c r="B18" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="C18" s="12">
         <v>0</v>
@@ -1714,12 +5378,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>16</v>
       </c>
       <c r="B19" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" s="9">
         <v>0</v>
@@ -1761,12 +5425,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>17</v>
       </c>
       <c r="B20" s="11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20" s="12">
         <v>0</v>
@@ -1808,12 +5472,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>18</v>
       </c>
       <c r="B21" s="8">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C21" s="9">
         <v>0</v>
@@ -1855,12 +5519,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>19</v>
       </c>
       <c r="B22" s="11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C22" s="12">
         <v>0</v>
@@ -1902,12 +5566,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>20</v>
       </c>
       <c r="B23" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23" s="9">
         <v>0</v>
@@ -1949,12 +5613,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>21</v>
       </c>
       <c r="B24" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="12">
         <v>0</v>
@@ -1996,12 +5660,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>22</v>
       </c>
       <c r="B25" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -2043,12 +5707,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>23</v>
       </c>
       <c r="B26" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="12">
         <v>0</v>
@@ -2090,12 +5754,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>24</v>
       </c>
       <c r="B27" s="8">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -2137,12 +5801,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>25</v>
       </c>
       <c r="B28" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" s="12">
         <v>0</v>
@@ -2184,12 +5848,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>26</v>
       </c>
       <c r="B29" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="9">
         <v>0</v>
@@ -2231,12 +5895,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>27</v>
       </c>
       <c r="B30" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="12">
         <v>0</v>
@@ -2278,12 +5942,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>28</v>
       </c>
       <c r="B31" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="9">
         <v>0</v>
@@ -2325,12 +5989,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>29</v>
       </c>
       <c r="B32" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="12">
         <v>0</v>
@@ -2372,12 +6036,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>30</v>
       </c>
       <c r="B33" s="8">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -2419,12 +6083,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>31</v>
       </c>
       <c r="B34" s="11">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="C34" s="12">
         <v>0</v>
@@ -2466,12 +6130,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>32</v>
       </c>
       <c r="B35" s="8">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -2513,12 +6177,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>33</v>
       </c>
       <c r="B36" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" s="12">
         <v>0</v>
@@ -2560,12 +6224,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>34</v>
       </c>
       <c r="B37" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37" s="9">
         <v>0</v>
@@ -2607,12 +6271,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>35</v>
       </c>
       <c r="B38" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38" s="12">
         <v>0</v>
@@ -2654,12 +6318,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>36</v>
       </c>
       <c r="B39" s="8">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C39" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
tested multiple_run_results and its looking gooood
</commit_message>
<xml_diff>
--- a/raw_inputs/vent.xlsx
+++ b/raw_inputs/vent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="tec_params" sheetId="1" r:id="rId1"/>
@@ -889,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -1112,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="11">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -1159,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="8">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -1206,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="11">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
@@ -1253,7 +1253,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="8">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -1300,7 +1300,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="11">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C10" s="12">
         <v>0</v>
@@ -1347,7 +1347,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="8">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
@@ -1394,7 +1394,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="11">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C12" s="12">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="8">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
@@ -1488,7 +1488,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="11">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C14" s="12">
         <v>0</v>
@@ -1535,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1582,7 +1582,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="12">
         <v>0</v>
@@ -1629,7 +1629,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
@@ -1676,7 +1676,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="11">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="C18" s="12">
         <v>0</v>
@@ -2719,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5">
-        <v>11.41</v>
+        <v>11</v>
       </c>
       <c r="C4" s="14">
         <v>1</v>
@@ -2895,7 +2895,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8">
-        <v>11.41</v>
+        <v>11</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -3694,7 +3694,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="11">
-        <v>5.41</v>
+        <v>7</v>
       </c>
       <c r="C22" s="12">
         <v>0</v>
@@ -3741,7 +3741,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="8">
-        <v>5.41</v>
+        <v>7</v>
       </c>
       <c r="C23" s="9">
         <v>0</v>
@@ -3788,7 +3788,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="11">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="12">
         <v>0</v>
@@ -3835,7 +3835,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="8">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -3882,7 +3882,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="11">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="12">
         <v>0</v>
@@ -3929,7 +3929,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="8">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -3976,7 +3976,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="11">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="12">
         <v>0</v>
@@ -4023,7 +4023,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="8">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="9">
         <v>0</v>
@@ -4070,7 +4070,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="11">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="12">
         <v>0</v>
@@ -4117,7 +4117,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="8">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="9">
         <v>0</v>
@@ -4164,7 +4164,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="11">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C32" s="12">
         <v>0</v>
@@ -4211,7 +4211,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="8">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -4258,7 +4258,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="11">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C34" s="12">
         <v>0</v>
@@ -4305,7 +4305,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="8">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -4352,7 +4352,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="11">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C36" s="12">
         <v>0</v>
@@ -4549,8 +4549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4772,7 +4772,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -4819,7 +4819,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="8">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -4866,7 +4866,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
@@ -4913,7 +4913,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="8">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -4960,7 +4960,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="12">
         <v>0</v>
@@ -5007,7 +5007,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="8">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
@@ -5054,7 +5054,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="12">
         <v>0</v>
@@ -5101,7 +5101,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="8">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
@@ -5148,7 +5148,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="12">
         <v>0</v>
@@ -5336,7 +5336,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C18" s="12">
         <v>0</v>
@@ -6041,7 +6041,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="8">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -6088,7 +6088,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="11">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="C34" s="12">
         <v>0</v>
@@ -6135,7 +6135,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="8">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
pareto run fixed + result sheet
</commit_message>
<xml_diff>
--- a/raw_inputs/vent.xlsx
+++ b/raw_inputs/vent.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_ABC70DE12AFBCFB532DBD6BAED603B6480CFADAD" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4732452F-CFC8-46F2-A2A5-6BEF1C76B2DC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tec_params" sheetId="1" r:id="rId1"/>
@@ -13,8 +14,9 @@
     <sheet name="n_50_table_1957" sheetId="4" r:id="rId4"/>
     <sheet name="n_50_table_1978" sheetId="5" r:id="rId5"/>
     <sheet name="n_50_table_1994" sheetId="6" r:id="rId6"/>
+    <sheet name="x_vent_table" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="54">
   <si>
     <t>cp_air</t>
   </si>
@@ -196,7 +198,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -285,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,6 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,16 +596,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -616,7 +619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -630,7 +633,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -644,7 +647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -661,16 +664,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -684,7 +687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -698,7 +701,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -712,7 +715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -726,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -740,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -754,7 +757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -768,7 +771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -782,7 +785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -796,7 +799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -811,20 +814,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -838,12 +841,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -852,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -866,7 +869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -886,51 +889,51 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.265625" customWidth="1"/>
+    <col min="6" max="6" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" customWidth="1"/>
+    <col min="12" max="12" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="C1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
       <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -968,7 +971,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>32</v>
@@ -1013,7 +1016,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1295,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="13">
         <v>7</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="10">
         <v>9</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1483,12 +1486,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="10">
         <v>11</v>
       </c>
       <c r="B14" s="11">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C14" s="12">
         <v>0</v>
@@ -1530,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="13">
         <v>13</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -1671,12 +1674,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="10">
         <v>15</v>
       </c>
       <c r="B18" s="11">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C18" s="12">
         <v>0</v>
@@ -1718,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="10">
         <v>17</v>
       </c>
@@ -1812,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="13">
         <v>19</v>
       </c>
@@ -1906,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -1953,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="10">
         <v>21</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -2047,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="10">
         <v>23</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="13">
         <v>25</v>
       </c>
@@ -2188,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="10">
         <v>27</v>
       </c>
@@ -2282,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -2329,12 +2332,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="10">
         <v>29</v>
       </c>
       <c r="B32" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="12">
         <v>0</v>
@@ -2376,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>30</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="13">
         <v>31</v>
       </c>
@@ -2470,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -2517,12 +2520,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="10">
         <v>33</v>
       </c>
       <c r="B36" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="12">
         <v>0</v>
@@ -2564,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="10">
         <v>35</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="7">
         <v>36</v>
       </c>
@@ -2716,51 +2719,51 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M34" activeCellId="3" sqref="M24 M26 M32 M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.265625" customWidth="1"/>
+    <col min="6" max="6" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" customWidth="1"/>
+    <col min="12" max="12" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="C1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="14"/>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
       <c r="N1" s="14"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>32</v>
@@ -2843,7 +2846,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -2890,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -3031,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -3078,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -3125,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="13">
         <v>7</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="10">
         <v>9</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -3313,12 +3316,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="10">
         <v>11</v>
       </c>
       <c r="B14" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="12">
         <v>0</v>
@@ -3360,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="13">
         <v>13</v>
       </c>
@@ -3454,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -3501,12 +3504,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="10">
         <v>15</v>
       </c>
       <c r="B18" s="11">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C18" s="12">
         <v>0</v>
@@ -3548,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -3595,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="10">
         <v>17</v>
       </c>
@@ -3642,7 +3645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -3689,7 +3692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="13">
         <v>19</v>
       </c>
@@ -3736,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -3783,7 +3786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="10">
         <v>21</v>
       </c>
@@ -3830,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="10">
         <v>23</v>
       </c>
@@ -3924,7 +3927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -3971,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="13">
         <v>25</v>
       </c>
@@ -4018,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -4065,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="10">
         <v>27</v>
       </c>
@@ -4112,7 +4115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -4159,7 +4162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="10">
         <v>29</v>
       </c>
@@ -4206,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>30</v>
       </c>
@@ -4253,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="13">
         <v>31</v>
       </c>
@@ -4300,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -4347,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="10">
         <v>33</v>
       </c>
@@ -4394,7 +4397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -4441,7 +4444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="10">
         <v>35</v>
       </c>
@@ -4488,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="7">
         <v>36</v>
       </c>
@@ -4546,51 +4549,51 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.265625" customWidth="1"/>
+    <col min="6" max="6" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" customWidth="1"/>
+    <col min="12" max="12" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="C1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="14"/>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
       <c r="N1" s="14"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -4628,7 +4631,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>32</v>
@@ -4673,7 +4676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -4720,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -4767,7 +4770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -4814,7 +4817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -4908,7 +4911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -4955,7 +4958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="13">
         <v>7</v>
       </c>
@@ -5002,7 +5005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -5049,7 +5052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="10">
         <v>9</v>
       </c>
@@ -5096,7 +5099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -5143,7 +5146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="10">
         <v>11</v>
       </c>
@@ -5190,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -5237,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="13">
         <v>13</v>
       </c>
@@ -5284,7 +5287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -5331,7 +5334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="10">
         <v>15</v>
       </c>
@@ -5378,7 +5381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -5425,7 +5428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="10">
         <v>17</v>
       </c>
@@ -5472,7 +5475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -5519,7 +5522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="13">
         <v>19</v>
       </c>
@@ -5566,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -5613,7 +5616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="10">
         <v>21</v>
       </c>
@@ -5660,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -5707,7 +5710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="10">
         <v>23</v>
       </c>
@@ -5754,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -5801,7 +5804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="13">
         <v>25</v>
       </c>
@@ -5848,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -5895,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="10">
         <v>27</v>
       </c>
@@ -5942,7 +5945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -5989,7 +5992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="10">
         <v>29</v>
       </c>
@@ -6036,7 +6039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>30</v>
       </c>
@@ -6083,7 +6086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="13">
         <v>31</v>
       </c>
@@ -6130,7 +6133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -6177,7 +6180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="10">
         <v>33</v>
       </c>
@@ -6224,7 +6227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -6271,7 +6274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="10">
         <v>35</v>
       </c>
@@ -6318,7 +6321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="7">
         <v>36</v>
       </c>
@@ -6373,4 +6376,297 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="15"/>
+      <c r="B2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>